<commit_message>
edited and cleared after testing import
</commit_message>
<xml_diff>
--- a/python/new_import.xlsx
+++ b/python/new_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\rs_intern\rs-intern\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4C7E7E-71E2-4878-B085-3C742E6B775A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF38A4E-21D9-4832-AC54-AFB60FD8122E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:BB1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
cleaned after testing functionality of build_import.py & scrape_ndc.py
</commit_message>
<xml_diff>
--- a/python/new_import.xlsx
+++ b/python/new_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\rs_intern\rs-intern\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF38A4E-21D9-4832-AC54-AFB60FD8122E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A8145-7BF9-4CE5-AC43-59257CA2C3D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:BB1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>